<commit_message>
Modifying view to match new model
</commit_message>
<xml_diff>
--- a/public/uploads/sheet/attachment/1/Book1.xlsx
+++ b/public/uploads/sheet/attachment/1/Book1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\toaster\homes\c\h\chenhongquan\nt\AccountSettings\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\toaster\homes\g\u\guangzhou92\nt\AccountSettings\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -336,22 +336,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>123</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E3">
-        <v>1</v>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifying Cucumber for new iteration
</commit_message>
<xml_diff>
--- a/public/uploads/sheet/attachment/1/Book1.xlsx
+++ b/public/uploads/sheet/attachment/1/Book1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\toaster\homes\c\h\chenhongquan\nt\AccountSettings\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\toaster\homes\g\u\guangzhou92\nt\AccountSettings\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,80 +23,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>LAST NAME</t>
-  </si>
-  <si>
-    <t>FIRST NAME</t>
-  </si>
-  <si>
-    <t>UIN</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>COLLEGE</t>
-  </si>
-  <si>
-    <t>FULL ACADEMIC UNIT NAME</t>
-  </si>
-  <si>
-    <t>DEGREE</t>
-  </si>
-  <si>
-    <t>POSITION</t>
-  </si>
-  <si>
-    <t>Abdelrahman</t>
-  </si>
-  <si>
-    <t>Nahed</t>
-  </si>
-  <si>
-    <t>nrahman@tamu.edu</t>
-  </si>
-  <si>
-    <t>Education and Human Development</t>
-  </si>
-  <si>
-    <t>Educational Administration and Human Resource Development</t>
-  </si>
-  <si>
-    <t>Doctoral</t>
-  </si>
-  <si>
-    <t>Representative</t>
-  </si>
-  <si>
-    <t>Abell</t>
-  </si>
-  <si>
-    <t>Lydia</t>
-  </si>
-  <si>
-    <t>lydiakathleenabell@email.tamu.edu</t>
-  </si>
-  <si>
-    <t>Liberal Arts</t>
-  </si>
-  <si>
-    <t>Performance Studies</t>
-  </si>
-  <si>
-    <t>Master's</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,25 +33,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,16 +54,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,93 +336,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4">
-        <v>222000917</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4">
-        <v>523005938</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>